<commit_message>
Quality of User Interface Upgrade and some checks
</commit_message>
<xml_diff>
--- a/public/docs/MultiplePersonalDataSheetFormat.xlsx
+++ b/public/docs/MultiplePersonalDataSheetFormat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0EEE43-7D9D-4DD4-8B0F-FC2B31B18E84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95046762-CFC2-4553-9A01-03037B70BB40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" firstSheet="1" activeTab="3" xr2:uid="{5B9E9E34-6855-468F-AE91-E64715C6457F}"/>
   </bookViews>
@@ -19,6 +19,9 @@
     <sheet name="CivilServiceElegibility" sheetId="4" r:id="rId4"/>
     <sheet name="WorkExperience" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">personalInformation!$G$3:$G$205</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="282">
   <si>
     <t>Surname</t>
   </si>
@@ -76,12 +79,6 @@
     <t>AGENCY EMPLOYEE NO.</t>
   </si>
   <si>
-    <t>Filipino</t>
-  </si>
-  <si>
-    <t>Dual Citizenship</t>
-  </si>
-  <si>
     <t>If Dual Citizenship please indicate the country</t>
   </si>
   <si>
@@ -796,9 +793,6 @@
     <t>Scholarship/ Academic Honors Received</t>
   </si>
   <si>
-    <t>Period Of Attendance</t>
-  </si>
-  <si>
     <t>Elementary</t>
   </si>
   <si>
@@ -838,9 +832,6 @@
     <t>Number</t>
   </si>
   <si>
-    <t>Date Of Validity</t>
-  </si>
-  <si>
     <t>Work Experience</t>
   </si>
   <si>
@@ -872,6 +863,21 @@
   </si>
   <si>
     <t>Sex(M,F)</t>
+  </si>
+  <si>
+    <t>Filipino (Y or N)</t>
+  </si>
+  <si>
+    <t>Dual Citizenship (Y or N)</t>
+  </si>
+  <si>
+    <t>Period Of Attendance (MM/DD/YYYY)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (MM/DD/YYYY)</t>
+  </si>
+  <si>
+    <t>Date Of Validity  (MM/DD/YYYY)</t>
   </si>
 </sst>
 </file>
@@ -923,7 +929,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -989,15 +995,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1021,12 +1018,60 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1037,38 +1082,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1078,10 +1096,46 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1562,7 +1616,7 @@
   <dimension ref="A1:AL205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,8 +1636,8 @@
     <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="22" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="42.28515625" customWidth="1"/>
     <col min="21" max="21" width="18.5703125" hidden="1" customWidth="1"/>
     <col min="22" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
@@ -1605,1538 +1659,1544 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="A1" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="H2" s="13" t="s">
+      <c r="G2" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="O2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="P2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="Q2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="R2" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="T2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="S2" s="13" t="s">
+      <c r="U2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="V2" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="AA2" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="AB2" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="AD2" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE2" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="AF2" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="AG2" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="AH2" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="AI2" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="AJ2" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="AK2" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="AL2" s="7" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="19" t="s">
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="7"/>
+      <c r="AH3" s="7"/>
+      <c r="AI3" s="7"/>
+      <c r="AJ3" s="7"/>
+      <c r="AK3" s="7"/>
+      <c r="AL3" s="7"/>
+    </row>
+    <row r="4" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="W2" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="X2" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="Y2" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="Z2" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="AA2" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="AB2" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="AC2" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="AD2" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="AE2" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="AF2" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="AG2" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="AH2" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="AI2" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="AJ2" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="AK2" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="AL2" s="13" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
-        <v>1</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="20" t="s">
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="7"/>
+      <c r="AG4" s="7"/>
+      <c r="AH4" s="7"/>
+      <c r="AI4" s="7"/>
+      <c r="AJ4" s="7"/>
+      <c r="AK4" s="7"/>
+      <c r="AL4" s="7"/>
+    </row>
+    <row r="5" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="13"/>
-      <c r="Z3" s="13"/>
-      <c r="AA3" s="13"/>
-      <c r="AB3" s="13"/>
-      <c r="AC3" s="13"/>
-      <c r="AD3" s="13"/>
-      <c r="AE3" s="13"/>
-      <c r="AF3" s="13"/>
-      <c r="AG3" s="13"/>
-      <c r="AH3" s="13"/>
-      <c r="AI3" s="13"/>
-      <c r="AJ3" s="13"/>
-      <c r="AK3" s="13"/>
-      <c r="AL3" s="13"/>
-    </row>
-    <row r="4" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
-        <v>2</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="20" t="s">
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="7"/>
+      <c r="AI5" s="7"/>
+      <c r="AJ5" s="7"/>
+      <c r="AK5" s="7"/>
+      <c r="AL5" s="7"/>
+    </row>
+    <row r="6" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="V4" s="13"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13"/>
-      <c r="Z4" s="13"/>
-      <c r="AA4" s="13"/>
-      <c r="AB4" s="13"/>
-      <c r="AC4" s="13"/>
-      <c r="AD4" s="13"/>
-      <c r="AE4" s="13"/>
-      <c r="AF4" s="13"/>
-      <c r="AG4" s="13"/>
-      <c r="AH4" s="13"/>
-      <c r="AI4" s="13"/>
-      <c r="AJ4" s="13"/>
-      <c r="AK4" s="13"/>
-      <c r="AL4" s="13"/>
-    </row>
-    <row r="5" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
-        <v>3</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="20" t="s">
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="7"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="7"/>
+      <c r="AI6" s="7"/>
+      <c r="AJ6" s="7"/>
+      <c r="AK6" s="7"/>
+      <c r="AL6" s="7"/>
+    </row>
+    <row r="7" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="13"/>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="13"/>
-      <c r="AD5" s="13"/>
-      <c r="AE5" s="13"/>
-      <c r="AF5" s="13"/>
-      <c r="AG5" s="13"/>
-      <c r="AH5" s="13"/>
-      <c r="AI5" s="13"/>
-      <c r="AJ5" s="13"/>
-      <c r="AK5" s="13"/>
-      <c r="AL5" s="13"/>
-    </row>
-    <row r="6" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
-        <v>4</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="20" t="s">
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="7"/>
+      <c r="AI7" s="7"/>
+      <c r="AJ7" s="7"/>
+      <c r="AK7" s="7"/>
+      <c r="AL7" s="7"/>
+    </row>
+    <row r="8" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="13"/>
-      <c r="Z6" s="13"/>
-      <c r="AA6" s="13"/>
-      <c r="AB6" s="13"/>
-      <c r="AC6" s="13"/>
-      <c r="AD6" s="13"/>
-      <c r="AE6" s="13"/>
-      <c r="AF6" s="13"/>
-      <c r="AG6" s="13"/>
-      <c r="AH6" s="13"/>
-      <c r="AI6" s="13"/>
-      <c r="AJ6" s="13"/>
-      <c r="AK6" s="13"/>
-      <c r="AL6" s="13"/>
-    </row>
-    <row r="7" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
-        <v>5</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="20" t="s">
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="7"/>
+      <c r="AK8" s="7"/>
+      <c r="AL8" s="7"/>
+    </row>
+    <row r="9" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13"/>
-      <c r="Z7" s="13"/>
-      <c r="AA7" s="13"/>
-      <c r="AB7" s="13"/>
-      <c r="AC7" s="13"/>
-      <c r="AD7" s="13"/>
-      <c r="AE7" s="13"/>
-      <c r="AF7" s="13"/>
-      <c r="AG7" s="13"/>
-      <c r="AH7" s="13"/>
-      <c r="AI7" s="13"/>
-      <c r="AJ7" s="13"/>
-      <c r="AK7" s="13"/>
-      <c r="AL7" s="13"/>
-    </row>
-    <row r="8" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
-        <v>6</v>
-      </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="20" t="s">
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="7"/>
+      <c r="AH9" s="7"/>
+      <c r="AI9" s="7"/>
+      <c r="AJ9" s="7"/>
+      <c r="AK9" s="7"/>
+      <c r="AL9" s="7"/>
+    </row>
+    <row r="10" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="V8" s="13"/>
-      <c r="W8" s="13"/>
-      <c r="X8" s="13"/>
-      <c r="Y8" s="13"/>
-      <c r="Z8" s="13"/>
-      <c r="AA8" s="13"/>
-      <c r="AB8" s="13"/>
-      <c r="AC8" s="13"/>
-      <c r="AD8" s="13"/>
-      <c r="AE8" s="13"/>
-      <c r="AF8" s="13"/>
-      <c r="AG8" s="13"/>
-      <c r="AH8" s="13"/>
-      <c r="AI8" s="13"/>
-      <c r="AJ8" s="13"/>
-      <c r="AK8" s="13"/>
-      <c r="AL8" s="13"/>
-    </row>
-    <row r="9" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
-        <v>7</v>
-      </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="20" t="s">
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+      <c r="AG10" s="7"/>
+      <c r="AH10" s="7"/>
+      <c r="AI10" s="7"/>
+      <c r="AJ10" s="7"/>
+      <c r="AK10" s="7"/>
+      <c r="AL10" s="7"/>
+    </row>
+    <row r="11" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="V9" s="13"/>
-      <c r="W9" s="13"/>
-      <c r="X9" s="13"/>
-      <c r="Y9" s="13"/>
-      <c r="Z9" s="13"/>
-      <c r="AA9" s="13"/>
-      <c r="AB9" s="13"/>
-      <c r="AC9" s="13"/>
-      <c r="AD9" s="13"/>
-      <c r="AE9" s="13"/>
-      <c r="AF9" s="13"/>
-      <c r="AG9" s="13"/>
-      <c r="AH9" s="13"/>
-      <c r="AI9" s="13"/>
-      <c r="AJ9" s="13"/>
-      <c r="AK9" s="13"/>
-      <c r="AL9" s="13"/>
-    </row>
-    <row r="10" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
-        <v>8</v>
-      </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="20" t="s">
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="7"/>
+      <c r="AG11" s="7"/>
+      <c r="AH11" s="7"/>
+      <c r="AI11" s="7"/>
+      <c r="AJ11" s="7"/>
+      <c r="AK11" s="7"/>
+      <c r="AL11" s="7"/>
+    </row>
+    <row r="12" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="V10" s="13"/>
-      <c r="W10" s="13"/>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="13"/>
-      <c r="Z10" s="13"/>
-      <c r="AA10" s="13"/>
-      <c r="AB10" s="13"/>
-      <c r="AC10" s="13"/>
-      <c r="AD10" s="13"/>
-      <c r="AE10" s="13"/>
-      <c r="AF10" s="13"/>
-      <c r="AG10" s="13"/>
-      <c r="AH10" s="13"/>
-      <c r="AI10" s="13"/>
-      <c r="AJ10" s="13"/>
-      <c r="AK10" s="13"/>
-      <c r="AL10" s="13"/>
-    </row>
-    <row r="11" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
-        <v>9</v>
-      </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="V11" s="13"/>
-      <c r="W11" s="13"/>
-      <c r="X11" s="13"/>
-      <c r="Y11" s="13"/>
-      <c r="Z11" s="13"/>
-      <c r="AA11" s="13"/>
-      <c r="AB11" s="13"/>
-      <c r="AC11" s="13"/>
-      <c r="AD11" s="13"/>
-      <c r="AE11" s="13"/>
-      <c r="AF11" s="13"/>
-      <c r="AG11" s="13"/>
-      <c r="AH11" s="13"/>
-      <c r="AI11" s="13"/>
-      <c r="AJ11" s="13"/>
-      <c r="AK11" s="13"/>
-      <c r="AL11" s="13"/>
-    </row>
-    <row r="12" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
-        <v>10</v>
-      </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="13"/>
-      <c r="T12" s="13"/>
-      <c r="U12" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="V12" s="13"/>
-      <c r="W12" s="13"/>
-      <c r="X12" s="13"/>
-      <c r="Y12" s="13"/>
-      <c r="Z12" s="13"/>
-      <c r="AA12" s="13"/>
-      <c r="AB12" s="13"/>
-      <c r="AC12" s="13"/>
-      <c r="AD12" s="13"/>
-      <c r="AE12" s="13"/>
-      <c r="AF12" s="13"/>
-      <c r="AG12" s="13"/>
-      <c r="AH12" s="13"/>
-      <c r="AI12" s="13"/>
-      <c r="AJ12" s="13"/>
-      <c r="AK12" s="13"/>
-      <c r="AL12" s="13"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="7"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="7"/>
+      <c r="AE12" s="7"/>
+      <c r="AF12" s="7"/>
+      <c r="AG12" s="7"/>
+      <c r="AH12" s="7"/>
+      <c r="AI12" s="7"/>
+      <c r="AJ12" s="7"/>
+      <c r="AK12" s="7"/>
+      <c r="AL12" s="7"/>
     </row>
     <row r="13" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U13" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U14" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U15" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U16" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U17" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U18" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U19" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U20" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U21" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U22" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U23" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U24" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U25" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U26" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U27" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U28" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U29" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U30" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U31" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U32" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U33" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U34" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U35" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U36" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U37" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U38" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U39" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U40" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U41" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U42" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U43" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U44" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U45" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U46" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U47" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U48" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U49" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U50" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U51" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U52" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U53" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U54" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U55" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U56" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U57" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U58" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U59" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U60" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U61" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U62" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U63" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U64" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U65" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U66" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="67" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U67" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U68" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U69" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U70" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U71" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U72" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="73" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U73" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="74" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U74" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="75" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U75" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="76" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U76" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="77" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U77" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="78" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U78" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="79" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U79" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="80" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U80" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="81" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U81" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="82" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U82" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="83" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U83" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="84" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U84" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="85" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U85" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="86" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U86" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="87" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U87" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="88" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U88" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="89" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U89" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="90" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U90" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="91" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U91" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="92" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U92" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="93" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U93" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="94" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U94" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="95" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U95" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="96" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U96" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="97" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U97" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="98" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U98" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="99" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U99" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="100" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U100" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="101" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U101" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="102" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U102" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U103" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="104" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U104" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="105" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U105" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="106" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U106" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="107" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U107" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="108" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U108" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="109" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U109" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="110" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U110" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="111" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U111" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="112" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U112" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="113" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U113" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="114" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U114" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="115" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U115" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="116" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U116" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="117" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U117" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="118" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U118" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="119" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U119" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="120" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U120" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="121" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U121" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="122" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U122" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="123" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U123" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="124" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U124" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="125" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U125" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="126" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U126" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="127" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U127" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="128" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U128" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="129" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U129" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="130" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U130" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="131" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U131" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="132" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U132" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="133" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U133" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="134" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U134" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="135" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U135" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="136" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U136" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="137" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U137" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="138" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U138" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="139" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U139" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="140" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U140" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="141" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U141" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="142" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U142" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="143" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U143" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="144" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U144" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="145" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U145" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="146" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U146" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="147" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U147" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="148" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U148" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="149" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U149" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="150" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U150" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="151" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U151" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="152" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U152" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="153" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U153" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="154" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U154" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="155" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U155" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="156" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U156" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="157" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U157" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="158" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U158" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="159" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U159" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="160" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U160" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="161" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U161" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="162" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U162" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="163" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U163" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="164" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U164" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="165" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U165" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="166" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U166" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="167" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U167" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="168" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U168" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="169" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U169" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="170" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U170" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="171" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U171" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="172" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U172" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="173" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U173" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="174" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U174" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="175" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U175" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="176" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U176" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="177" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U177" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="178" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U178" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="179" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U179" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="180" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U180" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="181" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U181" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="182" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U182" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="183" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U183" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="184" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U184" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="185" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U185" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="186" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U186" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="187" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U187" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="188" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U188" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="189" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U189" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="190" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U190" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="191" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U191" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="192" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U192" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="193" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U193" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="194" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U194" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="195" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U195" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="196" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U196" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="197" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U197" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="198" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U198" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="199" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U199" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="200" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U200" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="201" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U201" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="202" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U202" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="203" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U203" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="204" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U204" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="205" spans="21:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U205" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T3:T1048576" xr:uid="{228B10C2-981F-4789-9A7E-BDB5F3C03DF6}">
       <formula1>$U$3:$U$205</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G1048576 G3" xr:uid="{721EDD25-D6CD-47B1-97BB-B939E6B2773E}">
+      <formula1>"M,F"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R1048576 S3:S1048576" xr:uid="{BACA2DD6-ADEA-4D24-A390-B7D797FB0668}">
+      <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -3345,7 +3405,8 @@
     <hyperlink ref="U3" r:id="rId203" display="http://www.state.gov/p/eur/ci/al/" xr:uid="{3FEE0289-C72B-4F3E-8F97-4F6AC7B37863}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId204"/>
+  <pageSetup orientation="portrait" r:id="rId204"/>
+  <drawing r:id="rId205"/>
 </worksheet>
 </file>
 
@@ -3381,305 +3442,305 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+    </row>
+    <row r="2" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="17"/>
+      <c r="J2" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="M2" s="16"/>
+      <c r="N2" s="17"/>
+      <c r="P2" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="17"/>
+    </row>
+    <row r="3" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="21" t="s">
-        <v>235</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="11"/>
-      <c r="J2" s="22" t="s">
+      <c r="F3" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="N3" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="L2" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="M2" s="10"/>
-      <c r="N2" s="11"/>
-      <c r="P2" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="11"/>
-    </row>
-    <row r="3" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13" t="s">
+      <c r="O3" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="P3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="Q3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="R3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="13" t="s">
+    </row>
+    <row r="4" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="R3" s="13" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+    </row>
+    <row r="5" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
-        <v>1</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-    </row>
-    <row r="5" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
-        <v>2</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
     </row>
     <row r="6" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
+      <c r="A6" s="7">
         <v>3</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
     </row>
     <row r="7" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="A7" s="7">
         <v>4</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
     </row>
     <row r="8" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
+      <c r="A8" s="7">
         <v>5</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
     </row>
     <row r="9" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
+      <c r="A9" s="7">
         <v>6</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
     </row>
     <row r="10" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
+      <c r="A10" s="7">
         <v>7</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
     </row>
     <row r="11" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
+      <c r="A11" s="7">
         <v>8</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
     </row>
     <row r="12" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
+      <c r="A12" s="7">
         <v>9</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
     </row>
     <row r="13" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+      <c r="A13" s="7">
         <v>10</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
     </row>
     <row r="14" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3889,8 +3950,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AJ13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="AG1" sqref="AF1:AG1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3898,592 +3959,592 @@
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13" customWidth="1"/>
+    <col min="4" max="5" width="18.28515625" customWidth="1"/>
     <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13" customWidth="1"/>
+    <col min="11" max="12" width="17.42578125" customWidth="1"/>
     <col min="13" max="13" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="13" customWidth="1"/>
+    <col min="18" max="19" width="18.5703125" customWidth="1"/>
     <col min="20" max="20" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="13" customWidth="1"/>
+    <col min="25" max="26" width="18.140625" customWidth="1"/>
     <col min="27" max="27" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="15" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="13" customWidth="1"/>
+    <col min="32" max="33" width="17.140625" customWidth="1"/>
     <col min="34" max="34" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="37.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="A1" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="E2" s="18"/>
+      <c r="I2" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="J2" s="17"/>
+      <c r="K2" s="21" t="s">
+        <v>279</v>
+      </c>
+      <c r="L2" s="14"/>
+      <c r="P2" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="S2" s="18"/>
+      <c r="W2" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="E2" s="9"/>
-      <c r="I2" s="21" t="s">
+      <c r="X2" s="17"/>
+      <c r="Y2" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="Z2" s="18"/>
+      <c r="AD2" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="L2" s="9"/>
-      <c r="P2" s="21" t="s">
-        <v>258</v>
-      </c>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="S2" s="9"/>
-      <c r="W2" s="21" t="s">
-        <v>259</v>
-      </c>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="Z2" s="9"/>
-      <c r="AD2" s="21" t="s">
-        <v>260</v>
-      </c>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="AG2" s="9"/>
+      <c r="AE2" s="17"/>
+      <c r="AF2" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="AG2" s="18"/>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="E3" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="F3" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="G3" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="H3" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="G3" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="L3" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="M3" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="N3" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="O3" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="N3" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="P3" s="13" t="s">
+      <c r="P3" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="R3" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="S3" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="R3" s="13" t="s">
+      <c r="T3" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="S3" s="13" t="s">
+      <c r="U3" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="T3" s="13" t="s">
+      <c r="V3" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="U3" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="V3" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="W3" s="13" t="s">
+      <c r="W3" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="Y3" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="X3" s="13" t="s">
+      <c r="Z3" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="Y3" s="13" t="s">
+      <c r="AA3" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="Z3" s="13" t="s">
+      <c r="AB3" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="AA3" s="13" t="s">
+      <c r="AC3" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="AB3" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="AC3" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="AD3" s="13" t="s">
+      <c r="AD3" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="AE3" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="AF3" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="AE3" s="13" t="s">
+      <c r="AG3" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="AF3" s="13" t="s">
+      <c r="AH3" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="AG3" s="13" t="s">
+      <c r="AI3" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="AH3" s="13" t="s">
+      <c r="AJ3" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="AI3" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="AJ3" s="13" t="s">
-        <v>254</v>
-      </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13"/>
-      <c r="Z4" s="13"/>
-      <c r="AA4" s="13"/>
-      <c r="AB4" s="13"/>
-      <c r="AC4" s="13"/>
-      <c r="AD4" s="13"/>
-      <c r="AE4" s="13"/>
-      <c r="AF4" s="13"/>
-      <c r="AG4" s="13"/>
-      <c r="AH4" s="13"/>
-      <c r="AI4" s="13"/>
-      <c r="AJ4" s="13"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="7"/>
+      <c r="AG4" s="7"/>
+      <c r="AH4" s="7"/>
+      <c r="AI4" s="7"/>
+      <c r="AJ4" s="7"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+      <c r="A5" s="7">
         <v>2</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="13"/>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="13"/>
-      <c r="AD5" s="13"/>
-      <c r="AE5" s="13"/>
-      <c r="AF5" s="13"/>
-      <c r="AG5" s="13"/>
-      <c r="AH5" s="13"/>
-      <c r="AI5" s="13"/>
-      <c r="AJ5" s="13"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="7"/>
+      <c r="AI5" s="7"/>
+      <c r="AJ5" s="7"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
+      <c r="A6" s="7">
         <v>3</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="13"/>
-      <c r="Z6" s="13"/>
-      <c r="AA6" s="13"/>
-      <c r="AB6" s="13"/>
-      <c r="AC6" s="13"/>
-      <c r="AD6" s="13"/>
-      <c r="AE6" s="13"/>
-      <c r="AF6" s="13"/>
-      <c r="AG6" s="13"/>
-      <c r="AH6" s="13"/>
-      <c r="AI6" s="13"/>
-      <c r="AJ6" s="13"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="7"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="7"/>
+      <c r="AI6" s="7"/>
+      <c r="AJ6" s="7"/>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="A7" s="7">
         <v>4</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13"/>
-      <c r="Z7" s="13"/>
-      <c r="AA7" s="13"/>
-      <c r="AB7" s="13"/>
-      <c r="AC7" s="13"/>
-      <c r="AD7" s="13"/>
-      <c r="AE7" s="13"/>
-      <c r="AF7" s="13"/>
-      <c r="AG7" s="13"/>
-      <c r="AH7" s="13"/>
-      <c r="AI7" s="13"/>
-      <c r="AJ7" s="13"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="7"/>
+      <c r="AI7" s="7"/>
+      <c r="AJ7" s="7"/>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
+      <c r="A8" s="7">
         <v>5</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
-      <c r="W8" s="13"/>
-      <c r="X8" s="13"/>
-      <c r="Y8" s="13"/>
-      <c r="Z8" s="13"/>
-      <c r="AA8" s="13"/>
-      <c r="AB8" s="13"/>
-      <c r="AC8" s="13"/>
-      <c r="AD8" s="13"/>
-      <c r="AE8" s="13"/>
-      <c r="AF8" s="13"/>
-      <c r="AG8" s="13"/>
-      <c r="AH8" s="13"/>
-      <c r="AI8" s="13"/>
-      <c r="AJ8" s="13"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="7"/>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
+      <c r="A9" s="7">
         <v>6</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="13"/>
-      <c r="V9" s="13"/>
-      <c r="W9" s="13"/>
-      <c r="X9" s="13"/>
-      <c r="Y9" s="13"/>
-      <c r="Z9" s="13"/>
-      <c r="AA9" s="13"/>
-      <c r="AB9" s="13"/>
-      <c r="AC9" s="13"/>
-      <c r="AD9" s="13"/>
-      <c r="AE9" s="13"/>
-      <c r="AF9" s="13"/>
-      <c r="AG9" s="13"/>
-      <c r="AH9" s="13"/>
-      <c r="AI9" s="13"/>
-      <c r="AJ9" s="13"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="7"/>
+      <c r="AH9" s="7"/>
+      <c r="AI9" s="7"/>
+      <c r="AJ9" s="7"/>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
+      <c r="A10" s="7">
         <v>7</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13"/>
-      <c r="W10" s="13"/>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="13"/>
-      <c r="Z10" s="13"/>
-      <c r="AA10" s="13"/>
-      <c r="AB10" s="13"/>
-      <c r="AC10" s="13"/>
-      <c r="AD10" s="13"/>
-      <c r="AE10" s="13"/>
-      <c r="AF10" s="13"/>
-      <c r="AG10" s="13"/>
-      <c r="AH10" s="13"/>
-      <c r="AI10" s="13"/>
-      <c r="AJ10" s="13"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+      <c r="AG10" s="7"/>
+      <c r="AH10" s="7"/>
+      <c r="AI10" s="7"/>
+      <c r="AJ10" s="7"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
+      <c r="A11" s="7">
         <v>8</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="W11" s="13"/>
-      <c r="X11" s="13"/>
-      <c r="Y11" s="13"/>
-      <c r="Z11" s="13"/>
-      <c r="AA11" s="13"/>
-      <c r="AB11" s="13"/>
-      <c r="AC11" s="13"/>
-      <c r="AD11" s="13"/>
-      <c r="AE11" s="13"/>
-      <c r="AF11" s="13"/>
-      <c r="AG11" s="13"/>
-      <c r="AH11" s="13"/>
-      <c r="AI11" s="13"/>
-      <c r="AJ11" s="13"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="7"/>
+      <c r="AG11" s="7"/>
+      <c r="AH11" s="7"/>
+      <c r="AI11" s="7"/>
+      <c r="AJ11" s="7"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
+      <c r="A12" s="7">
         <v>9</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="13"/>
-      <c r="T12" s="13"/>
-      <c r="U12" s="13"/>
-      <c r="V12" s="13"/>
-      <c r="W12" s="13"/>
-      <c r="X12" s="13"/>
-      <c r="Y12" s="13"/>
-      <c r="Z12" s="13"/>
-      <c r="AA12" s="13"/>
-      <c r="AB12" s="13"/>
-      <c r="AC12" s="13"/>
-      <c r="AD12" s="13"/>
-      <c r="AE12" s="13"/>
-      <c r="AF12" s="13"/>
-      <c r="AG12" s="13"/>
-      <c r="AH12" s="13"/>
-      <c r="AI12" s="13"/>
-      <c r="AJ12" s="13"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="7"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="7"/>
+      <c r="AE12" s="7"/>
+      <c r="AF12" s="7"/>
+      <c r="AG12" s="7"/>
+      <c r="AH12" s="7"/>
+      <c r="AI12" s="7"/>
+      <c r="AJ12" s="7"/>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+      <c r="A13" s="7">
         <v>10</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
-      <c r="U13" s="13"/>
-      <c r="V13" s="13"/>
-      <c r="W13" s="13"/>
-      <c r="X13" s="13"/>
-      <c r="Y13" s="13"/>
-      <c r="Z13" s="13"/>
-      <c r="AA13" s="13"/>
-      <c r="AB13" s="13"/>
-      <c r="AC13" s="13"/>
-      <c r="AD13" s="13"/>
-      <c r="AE13" s="13"/>
-      <c r="AF13" s="13"/>
-      <c r="AG13" s="13"/>
-      <c r="AH13" s="13"/>
-      <c r="AI13" s="13"/>
-      <c r="AJ13" s="13"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="7"/>
+      <c r="AE13" s="7"/>
+      <c r="AF13" s="7"/>
+      <c r="AG13" s="7"/>
+      <c r="AH13" s="7"/>
+      <c r="AI13" s="7"/>
+      <c r="AJ13" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -4514,7 +4575,7 @@
   <dimension ref="A1:R205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4523,244 +4584,249 @@
     <col min="3" max="3" width="16.42578125" style="1"/>
     <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="F1" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="H1" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="I1" s="18"/>
+    </row>
+    <row r="2" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11"/>
-      <c r="H1" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="I1" s="9"/>
-    </row>
-    <row r="2" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="12" t="s">
+      <c r="G2" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="F2" s="13" t="s">
+      <c r="H2" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>269</v>
+      <c r="I2" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+        <v>235</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
       <c r="O2" t="s">
-        <v>237</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
+        <v>235</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>237</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>237</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>237</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>237</v>
+      <c r="B3" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>235</v>
       </c>
       <c r="J3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="M3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="N3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="O3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="P3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="Q3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="R3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+      <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
+      <c r="B4" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
+      <c r="B5" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
+      <c r="B6" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
+      <c r="B7" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
+      <c r="A8" s="7">
         <v>6</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
+      <c r="B8" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
+      <c r="A9" s="7">
         <v>7</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
+      <c r="B9" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
+      <c r="A10" s="7">
         <v>8</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
+      <c r="B10" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
+      <c r="A11" s="7">
         <v>9</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
+      <c r="B11" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
+      <c r="A12" s="7">
         <v>10</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
+      <c r="B12" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4957,21 +5023,21 @@
     <row r="205" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4982,7 +5048,7 @@
   <dimension ref="A1:R205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E3"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4999,163 +5065,233 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="20" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="22" t="s">
+        <v>267</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="H2" s="19"/>
+      <c r="I2" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" t="s">
+        <v>235</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+    </row>
+    <row r="3" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11"/>
-      <c r="I1" s="5"/>
-    </row>
-    <row r="2" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
-        <v>279</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="15" t="s">
+      <c r="H3" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>272</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>273</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" t="s">
-        <v>237</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-    </row>
-    <row r="3" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
-        <v>250</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" t="s">
-        <v>274</v>
-      </c>
-      <c r="H3" t="s">
-        <v>275</v>
-      </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="17"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
       <c r="K3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="M3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="N3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="O3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="P3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="Q3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="R3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>